<commit_message>
Adicionado dicionário de dados da tabela item_orcamento
</commit_message>
<xml_diff>
--- a/Documentação/Banco de dados/Dicionário de Dados/Dicionário de Dados - Samaforte.xlsx
+++ b/Documentação/Banco de dados/Dicionário de Dados/Dicionário de Dados - Samaforte.xlsx
@@ -14,6 +14,7 @@
     <sheet state="visible" name="D.D - perfil" sheetId="9" r:id="rId12"/>
     <sheet state="visible" name="D.D - relatorio" sheetId="10" r:id="rId13"/>
     <sheet state="visible" name="D.D - perfil_menu" sheetId="11" r:id="rId14"/>
+    <sheet state="visible" name="D.D - item_orcamento" sheetId="12" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="150">
   <si>
     <t>Tabela</t>
   </si>
@@ -467,6 +468,47 @@
   <si>
     <t>Código de identificação da relação 
 entre um perfil e um menu.</t>
+  </si>
+  <si>
+    <t>Código de identificação
+ do item do orçamento.</t>
+  </si>
+  <si>
+    <t>id_produto</t>
+  </si>
+  <si>
+    <t>Código de identificação 
+do produto citado no item.</t>
+  </si>
+  <si>
+    <t>Código de identificação 
+do orçamento a qual 
+o item pertence.</t>
+  </si>
+  <si>
+    <t>Quantidade do produto desejado.</t>
+  </si>
+  <si>
+    <t>preco_unitario</t>
+  </si>
+  <si>
+    <t>Preço uniário do produto.</t>
+  </si>
+  <si>
+    <t>Preço = 
+Preço Unitário * Quantidade.</t>
+  </si>
+  <si>
+    <t>dataHora</t>
+  </si>
+  <si>
+    <t>Data e hora da criação do item.</t>
+  </si>
+  <si>
+    <t>statusVenda</t>
+  </si>
+  <si>
+    <t>Status da Venda do item.</t>
   </si>
 </sst>
 </file>
@@ -627,6 +669,10 @@
 </file>
 
 <file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1373,6 +1419,201 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="13.38"/>
+    <col customWidth="1" min="3" max="3" width="16.38"/>
+    <col customWidth="1" min="4" max="5" width="13.88"/>
+    <col customWidth="1" min="6" max="6" width="11.38"/>
+    <col customWidth="1" min="7" max="7" width="26.38"/>
+  </cols>
+  <sheetData>
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="B2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="7"/>
+      <c r="C4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="7"/>
+      <c r="C5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="7"/>
+      <c r="C6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="7"/>
+      <c r="C7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="7"/>
+      <c r="C8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="7"/>
+      <c r="C9" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="5"/>
+      <c r="C10" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:B10"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="1.0" right="1.0" top="1.0"/>
+  <pageSetup fitToHeight="0" paperSize="9" orientation="portrait" pageOrder="overThenDown"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>

</xml_diff>